<commit_message>
chore: add monthly employment outputs
</commit_message>
<xml_diff>
--- a/data/master/employment_master.xlsx
+++ b/data/master/employment_master.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -578,7 +578,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -624,7 +624,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -762,7 +762,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -808,7 +808,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -992,7 +992,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1452,7 +1452,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1728,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1774,7 +1774,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -1958,7 +1958,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2142,7 +2142,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2280,7 +2280,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2510,7 +2510,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2556,7 +2556,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2602,7 +2602,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2694,7 +2694,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2740,7 +2740,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -2995,7 +2995,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3041,7 +3041,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3179,7 +3179,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3271,7 +3271,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3455,7 +3455,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3685,7 +3685,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3731,7 +3731,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3823,7 +3823,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3915,7 +3915,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4007,7 +4007,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4053,7 +4053,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4099,7 +4099,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4145,7 +4145,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4329,7 +4329,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4375,7 +4375,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4421,7 +4421,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4605,7 +4605,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4651,7 +4651,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4743,7 +4743,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4789,7 +4789,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4835,7 +4835,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4881,7 +4881,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -4973,7 +4973,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5019,7 +5019,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5065,7 +5065,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5182,7 +5182,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5274,7 +5274,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5320,7 +5320,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5366,7 +5366,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5412,7 +5412,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5458,7 +5458,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5550,7 +5550,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5596,7 +5596,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5642,7 +5642,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5688,7 +5688,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5734,7 +5734,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5826,7 +5826,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5872,7 +5872,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5918,7 +5918,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -5964,7 +5964,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6010,7 +6010,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6056,7 +6056,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6240,7 +6240,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6286,7 +6286,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6332,7 +6332,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6378,7 +6378,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6424,7 +6424,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6470,7 +6470,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6516,7 +6516,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6562,7 +6562,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6608,7 +6608,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6654,7 +6654,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6700,7 +6700,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6746,7 +6746,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6792,7 +6792,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6884,7 +6884,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -6976,7 +6976,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7022,7 +7022,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7068,7 +7068,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7114,7 +7114,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7160,7 +7160,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7206,7 +7206,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7252,7 +7252,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7298,7 +7298,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7344,7 +7344,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7390,7 +7390,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7507,7 +7507,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7553,7 +7553,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7599,7 +7599,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7645,7 +7645,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7691,7 +7691,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7737,7 +7737,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7783,7 +7783,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7829,7 +7829,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7875,7 +7875,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7921,7 +7921,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -7967,7 +7967,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8013,7 +8013,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8059,7 +8059,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8105,7 +8105,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8151,7 +8151,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8197,7 +8197,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8243,7 +8243,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8289,7 +8289,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8335,7 +8335,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8381,7 +8381,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8427,7 +8427,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8473,7 +8473,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8519,7 +8519,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8565,7 +8565,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8611,7 +8611,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8703,7 +8703,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8749,7 +8749,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8795,7 +8795,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8841,7 +8841,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8887,7 +8887,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8933,7 +8933,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -8979,7 +8979,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9025,7 +9025,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9071,7 +9071,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9117,7 +9117,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9209,7 +9209,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9255,7 +9255,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9301,7 +9301,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9347,7 +9347,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9393,7 +9393,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9439,7 +9439,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9485,7 +9485,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9531,7 +9531,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9577,7 +9577,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9623,7 +9623,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9669,7 +9669,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9715,7 +9715,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9832,7 +9832,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9878,7 +9878,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9924,7 +9924,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -9970,7 +9970,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10016,7 +10016,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10062,7 +10062,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10108,7 +10108,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10154,7 +10154,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10200,7 +10200,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10246,7 +10246,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10292,7 +10292,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10338,7 +10338,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10384,7 +10384,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10430,7 +10430,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10476,7 +10476,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10522,7 +10522,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10568,7 +10568,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10614,7 +10614,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10660,7 +10660,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10706,7 +10706,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10752,7 +10752,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10798,7 +10798,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10844,7 +10844,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10890,7 +10890,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10936,7 +10936,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -10982,7 +10982,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11028,7 +11028,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11074,7 +11074,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11120,7 +11120,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11166,7 +11166,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11212,7 +11212,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11258,7 +11258,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11304,7 +11304,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11350,7 +11350,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11396,7 +11396,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11442,7 +11442,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11488,7 +11488,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11534,7 +11534,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11580,7 +11580,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11626,7 +11626,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11672,7 +11672,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11718,7 +11718,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11764,7 +11764,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11810,7 +11810,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11856,7 +11856,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11902,7 +11902,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11948,7 +11948,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -11994,7 +11994,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12040,7 +12040,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12137,7 +12137,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>13589</v>
+        <v>1435</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -12157,7 +12157,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12183,7 +12183,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>188692</v>
+        <v>2758</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -12203,7 +12203,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12229,7 +12229,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>56486</v>
+        <v>816</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -12249,7 +12249,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12275,27 +12275,27 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>68592</v>
+        <v>1054</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>주의</t>
+          <t>정상</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>주의</t>
+          <t>정상</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>주의</t>
+          <t>정상</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12321,7 +12321,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>91189</v>
+        <v>701</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -12341,7 +12341,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12367,7 +12367,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>32121</v>
+        <v>431</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -12387,7 +12387,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12413,7 +12413,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>59443</v>
+        <v>783</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -12433,7 +12433,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12459,7 +12459,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>129118</v>
+        <v>1144</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -12479,7 +12479,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12505,7 +12505,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120613</v>
+        <v>1683</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -12525,7 +12525,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12551,7 +12551,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>16095</v>
+        <v>134</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -12571,7 +12571,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12597,7 +12597,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>151272</v>
+        <v>1061</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -12617,7 +12617,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12643,27 +12643,27 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>421639</v>
+        <v>1361</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>관심</t>
+          <t>정상</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>관심</t>
+          <t>정상</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>정상</t>
+          <t>주의</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12709,7 +12709,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12755,7 +12755,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12801,7 +12801,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12847,7 +12847,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12893,7 +12893,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12939,7 +12939,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -12985,7 +12985,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13031,7 +13031,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13077,7 +13077,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13123,7 +13123,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13169,7 +13169,7 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13215,7 +13215,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13261,7 +13261,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13307,7 +13307,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13353,7 +13353,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13399,7 +13399,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13445,7 +13445,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13491,7 +13491,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13537,7 +13537,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13583,7 +13583,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13629,7 +13629,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13675,7 +13675,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13721,7 +13721,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13767,7 +13767,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13813,7 +13813,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13859,7 +13859,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13905,7 +13905,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13951,7 +13951,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -13997,7 +13997,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14043,7 +14043,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14089,7 +14089,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14135,7 +14135,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14181,7 +14181,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14227,7 +14227,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14273,7 +14273,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14319,7 +14319,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>
@@ -14365,7 +14365,7 @@
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>2026-02-12T23:04:40</t>
+          <t>2026-02-12T23:15:00</t>
         </is>
       </c>
     </row>

</xml_diff>